<commit_message>
feat: funcionalidade de análise de despesas
</commit_message>
<xml_diff>
--- a/gestao-financeira-usuario/usuarios.xlsx
+++ b/gestao-financeira-usuario/usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kantonis\desenv\api-gestao-financeira\gestao-financeira-usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07A886D-2332-48A7-B76A-97266838E86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4296308-CD58-4393-AAF4-38C8FF8FDC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nome</t>
   </si>
@@ -66,103 +66,31 @@
     <t>profissao 1</t>
   </si>
   <si>
-    <t>profissao 2</t>
-  </si>
-  <si>
-    <t>profissao 5</t>
-  </si>
-  <si>
-    <t>profissao 6</t>
-  </si>
-  <si>
-    <t>João A</t>
-  </si>
-  <si>
-    <t>João B</t>
-  </si>
-  <si>
-    <t>Maria A</t>
-  </si>
-  <si>
-    <t>Maria B</t>
-  </si>
-  <si>
-    <t>joao.a@email.com</t>
-  </si>
-  <si>
-    <t>joao.b@email.com</t>
-  </si>
-  <si>
-    <t>maria.a@email.com</t>
-  </si>
-  <si>
-    <t>maria.b@email.com</t>
-  </si>
-  <si>
     <t>rua 1</t>
   </si>
   <si>
-    <t>rua 2</t>
-  </si>
-  <si>
-    <t>rua 5</t>
-  </si>
-  <si>
-    <t>rua 4</t>
-  </si>
-  <si>
     <t>bairro 1</t>
   </si>
   <si>
-    <t>bairro 2</t>
-  </si>
-  <si>
-    <t>bairro 4</t>
-  </si>
-  <si>
-    <t>bairro 5</t>
-  </si>
-  <si>
     <t>cidade 1</t>
   </si>
   <si>
-    <t>cidade 2</t>
-  </si>
-  <si>
-    <t>cidade 4</t>
-  </si>
-  <si>
-    <t>cidade 5</t>
-  </si>
-  <si>
     <t>DF</t>
   </si>
   <si>
-    <t>PR</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
     <t>casa 1</t>
   </si>
   <si>
-    <t>casa 2</t>
-  </si>
-  <si>
-    <t>casa 4</t>
-  </si>
-  <si>
-    <t>casa 5</t>
-  </si>
-  <si>
-    <t>ativo</t>
-  </si>
-  <si>
-    <t>true</t>
+    <t>5561988771238</t>
+  </si>
+  <si>
+    <t>Cleber C</t>
+  </si>
+  <si>
+    <t>cleber@email.com</t>
+  </si>
+  <si>
+    <t>81232000</t>
   </si>
 </sst>
 </file>
@@ -229,13 +157,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -517,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,232 +462,135 @@
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14" style="4" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2">
-        <v>97000445510</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2">
-        <v>81230000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2">
+      <c r="C2">
+        <v>97000745531</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4">
         <v>100</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>5561988771234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>77000445511</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3">
-        <v>81240000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>200</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3">
-        <v>5561988771235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4">
-        <v>47000445512</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>81260000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <v>400</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4">
-        <v>5561988771237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <v>37000445513</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>81270000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5">
-        <v>500</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5">
-        <v>5561988771238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7289315C-D067-41EE-B8DE-784714AC806D}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{D8DC3EFF-CB75-48BD-865C-A00DA46752D1}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{079B2E04-0389-46AE-B500-74217303CB32}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{749A74E1-1C0C-42D4-8889-388FB381546E}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1DDA4C84-90FA-4173-AB04-A9519A993DF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>